<commit_message>
Update sửa thông tin
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/members.xlsx
+++ b/Hethongquanlylab/wwwroot/data/members.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\C#\Hethongquanlylab\Hethongquanlylab\wwwroot\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\Hethongquanly\Hethongquanlylab\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8602FA59-2706-4E28-BADD-01AE51CD8FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DB65BE-4401-478E-9412-73EF29AD7E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23040" yWindow="336" windowWidth="21600" windowHeight="11292" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>Key</t>
   </si>
@@ -81,28 +81,31 @@
     <t>default.jpg</t>
   </si>
   <si>
+    <t>Lã Quang Dương</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>2022-09-28</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>email@gmail.com</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Chưa có</t>
+  </si>
+  <si>
     <t>Ngô Xuân Hinh</t>
-  </si>
-  <si>
-    <t>Nam</t>
-  </si>
-  <si>
-    <t>2022-09-28</t>
-  </si>
-  <si>
-    <t>1,2</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>email@gmail.com</t>
-  </si>
-  <si>
-    <t>Chưa có</t>
   </si>
   <si>
     <t/>
@@ -552,9 +555,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
@@ -635,13 +644,13 @@
         <v>23</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K2" s="0" t="s">
         <v>24</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M2" s="0" t="s">
         <v>25</v>
@@ -664,7 +673,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>19</v>
@@ -676,16 +685,16 @@
         <v>21</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J3" s="0">
         <v>12</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M3" s="0" t="s">
         <v>25</v>
@@ -708,7 +717,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>19</v>
@@ -720,16 +729,16 @@
         <v>21</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J4" s="0">
         <v>12</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M4" s="0" t="s">
         <v>25</v>
@@ -752,7 +761,7 @@
         <v>323</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>19</v>
@@ -764,16 +773,16 @@
         <v>21</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J5" s="0">
         <v>12</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M5" s="0" t="s">
         <v>25</v>
@@ -796,7 +805,7 @@
         <v>3221</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>19</v>
@@ -808,16 +817,16 @@
         <v>21</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J6" s="0">
         <v>12</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M6" s="0" t="s">
         <v>25</v>
@@ -837,34 +846,34 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>21</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M7" s="0" t="s">
         <v>25</v>
@@ -884,40 +893,40 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>21</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O8" s="0" t="b">
         <v>0</v>
@@ -931,34 +940,34 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>21</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M9" s="0" t="s">
         <v>25</v>
@@ -978,13 +987,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>19</v>
@@ -996,16 +1005,16 @@
         <v>21</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M10" s="0" t="s">
         <v>25</v>
@@ -1025,40 +1034,40 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>21</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O11" s="0" t="b">
         <v>0</v>
@@ -1072,43 +1081,43 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>21</v>
       </c>
       <c r="H12" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="L12" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="I12" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="L12" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="M12" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N12" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O12" s="0" t="b">
         <v>0</v>
@@ -1122,37 +1131,37 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G13" s="0" t="s">
         <v>21</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M13" s="0" t="s">
         <v>25</v>
@@ -1172,37 +1181,37 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>21</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M14" s="0" t="s">
         <v>25</v>
@@ -1228,31 +1237,31 @@
         <v>17</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G15" s="0" t="s">
         <v>21</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M15" s="0" t="s">
         <v>25</v>
@@ -1272,37 +1281,37 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G16" s="0" t="s">
         <v>21</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M16" s="0" t="s">
         <v>25</v>
@@ -1322,37 +1331,37 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G17" s="0" t="s">
         <v>21</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M17" s="0" t="s">
         <v>25</v>
@@ -1372,37 +1381,37 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G18" s="0" t="s">
         <v>21</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M18" s="0" t="s">
         <v>25</v>
@@ -1422,37 +1431,37 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G19" s="0" t="s">
         <v>21</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M19" s="0" t="s">
         <v>25</v>
@@ -1472,37 +1481,37 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G20" s="0" t="s">
         <v>21</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M20" s="0" t="s">
         <v>25</v>
@@ -1522,37 +1531,37 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G21" s="0" t="s">
         <v>21</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M21" s="0" t="s">
         <v>25</v>
@@ -1572,37 +1581,37 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G22" s="0" t="s">
         <v>21</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M22" s="0" t="s">
         <v>25</v>
@@ -1622,13 +1631,13 @@
         <v>23</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>19</v>
@@ -1640,19 +1649,19 @@
         <v>21</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M23" s="0" t="s">
         <v>25</v>
@@ -1672,37 +1681,37 @@
         <v>24</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G24" s="0" t="s">
         <v>21</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M24" s="0" t="s">
         <v>25</v>
@@ -1722,13 +1731,13 @@
         <v>25</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>19</v>
@@ -1740,22 +1749,22 @@
         <v>21</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N25" s="0" t="s">
         <v>25</v>
@@ -1772,37 +1781,37 @@
         <v>26</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G26" s="0" t="s">
         <v>21</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M26" s="0" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Sửa thông tin cá nhân
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/members.xlsx
+++ b/Hethongquanlylab/wwwroot/data/members.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>Key</t>
   </si>
@@ -75,6 +75,9 @@
     <t>Qua PTBT?</t>
   </si>
   <si>
+    <t>N/A</t>
+  </si>
+  <si>
     <t>default.jpg</t>
   </si>
   <si>
@@ -87,9 +90,6 @@
     <t>2022-09-28</t>
   </si>
   <si>
-    <t>Điện tử Viễn Thông 123</t>
-  </si>
-  <si>
     <t>Đại học Bách Khoa Hà Nội</t>
   </si>
   <si>
@@ -99,7 +99,7 @@
     <t>email@gmail.com</t>
   </si>
   <si>
-    <t>Hải Dương 123</t>
+    <t xml:space="preserve">Hải Dương </t>
   </si>
   <si>
     <t>1,2</t>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>2022-09-08</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>999213</t>
@@ -625,20 +622,23 @@
       <c r="A2" s="0">
         <v>1</v>
       </c>
+      <c r="B2" s="0" t="s">
+        <v>16</v>
+      </c>
       <c r="C2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="0" t="s">
         <v>20</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="I2" s="0" t="s">
         <v>21</v>
@@ -651,6 +651,12 @@
       </c>
       <c r="L2" s="0" t="s">
         <v>24</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="O2" s="0" t="b">
         <v>0</v>
@@ -667,13 +673,13 @@
         <v>7</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>25</v>
@@ -711,13 +717,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G4" s="0" t="s">
         <v>25</v>
@@ -755,13 +761,13 @@
         <v>323</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>25</v>
@@ -799,13 +805,13 @@
         <v>3221</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>25</v>
@@ -843,13 +849,13 @@
         <v>28</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>29</v>
@@ -893,10 +899,10 @@
         <v>31</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>32</v>
@@ -937,13 +943,13 @@
         <v>38</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>39</v>
@@ -952,16 +958,16 @@
         <v>25</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="M9" s="0" t="s">
         <v>27</v>
@@ -981,34 +987,34 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>25</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="K10" s="0" t="s">
         <v>35</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="M10" s="0" t="s">
         <v>27</v>
@@ -1028,16 +1034,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>32</v>
@@ -1075,19 +1081,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>44</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>25</v>
@@ -1099,7 +1105,7 @@
         <v>21</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K12" s="0" t="s">
         <v>33</v>
@@ -1125,37 +1131,37 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="0" t="s">
+      <c r="E13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>48</v>
-      </c>
       <c r="G13" s="0" t="s">
         <v>25</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="M13" s="0" t="s">
         <v>27</v>
@@ -1175,37 +1181,37 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>50</v>
-      </c>
       <c r="G14" s="0" t="s">
         <v>25</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="M14" s="0" t="s">
         <v>27</v>
@@ -1228,34 +1234,34 @@
         <v>5021</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G15" s="0" t="s">
         <v>25</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="M15" s="0" t="s">
         <v>27</v>
@@ -1275,16 +1281,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>32</v>
@@ -1293,19 +1299,19 @@
         <v>25</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="M16" s="0" t="s">
         <v>27</v>
@@ -1325,40 +1331,40 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="D17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="0" t="s">
+      <c r="G17" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="M17" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="L17" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="M17" s="0" t="s">
-        <v>55</v>
       </c>
       <c r="N17" s="0" t="s">
         <v>27</v>
@@ -1375,40 +1381,40 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>57</v>
-      </c>
       <c r="G18" s="0" t="s">
         <v>25</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="N18" s="0" t="s">
         <v>27</v>
@@ -1425,37 +1431,37 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>59</v>
-      </c>
       <c r="G19" s="0" t="s">
         <v>25</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="M19" s="0" t="s">
         <v>27</v>
@@ -1475,37 +1481,37 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="D20" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>62</v>
-      </c>
       <c r="G20" s="0" t="s">
         <v>25</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="M20" s="0" t="s">
         <v>27</v>
@@ -1525,40 +1531,40 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G21" s="0" t="s">
         <v>25</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="N21" s="0" t="s">
         <v>27</v>
@@ -1575,37 +1581,37 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>64</v>
-      </c>
       <c r="E22" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G22" s="0" t="s">
         <v>25</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="M22" s="0" t="s">
         <v>27</v>
@@ -1625,37 +1631,37 @@
         <v>23</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="0" t="s">
-        <v>66</v>
-      </c>
       <c r="D23" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G23" s="0" t="s">
         <v>25</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="M23" s="0" t="s">
         <v>27</v>
@@ -1675,40 +1681,40 @@
         <v>24</v>
       </c>
       <c r="B24" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>64</v>
-      </c>
       <c r="E24" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G24" s="0" t="s">
         <v>25</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="N24" s="0" t="s">
         <v>27</v>
@@ -1725,40 +1731,40 @@
         <v>25</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G25" s="0" t="s">
         <v>25</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N25" s="0" t="s">
         <v>27</v>
@@ -1775,37 +1781,37 @@
         <v>26</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>64</v>
-      </c>
       <c r="E26" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G26" s="0" t="s">
         <v>25</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="M26" s="0" t="s">
         <v>27</v>
@@ -1828,34 +1834,34 @@
         <v>28</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G27" s="0" t="s">
         <v>25</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="M27" s="0" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Thông tin cá nhân
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/members.xlsx
+++ b/Hethongquanlylab/wwwroot/data/members.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\C#\Hethongquanlylab\Hethongquanlylab\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112976BC-8A86-416B-B8E4-6583859F09EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED408CA4-16B5-4CE5-BC0F-F072E51E659A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Key</t>
   </si>
@@ -75,76 +75,82 @@
     <t>Qua PTBT?</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Ngô Xuân Hinh.jpg</t>
+  </si>
+  <si>
+    <t>Ngô Xuân Hinh</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>2022-09-28</t>
+  </si>
+  <si>
+    <t>Khoa học máy tính 06</t>
+  </si>
+  <si>
+    <t>CNTT &amp; TT</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>23456@gmail.com</t>
+  </si>
+  <si>
+    <t>Phúc Yên, Vĩnh Phúc</t>
+  </si>
+  <si>
+    <t>Chưa có</t>
+  </si>
+  <si>
+    <t>default.jpg</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>999</t>
+  </si>
+  <si>
+    <t>2022-09-21</t>
+  </si>
+  <si>
+    <t>9999</t>
+  </si>
+  <si>
+    <t>45.png</t>
+  </si>
+  <si>
+    <t>2022-09-16</t>
+  </si>
+  <si>
+    <t>Khoa học máy tính</t>
+  </si>
+  <si>
+    <t>Đại học Bách Khoa Hà Nội</t>
+  </si>
+  <si>
+    <t>Ban Đào Tạo</t>
+  </si>
+  <si>
+    <t>Trưởng Ban</t>
+  </si>
+  <si>
+    <t>99999</t>
+  </si>
+  <si>
+    <t>2022-09-08</t>
+  </si>
+  <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>default.jpg</t>
-  </si>
-  <si>
-    <t>Ngô Xuân Hinh</t>
-  </si>
-  <si>
-    <t>Nam</t>
-  </si>
-  <si>
-    <t>2022-09-28</t>
-  </si>
-  <si>
-    <t>Đại học Bách Khoa Hà Nội</t>
-  </si>
-  <si>
-    <t>0996336668</t>
-  </si>
-  <si>
-    <t>email@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hải Dương </t>
-  </si>
-  <si>
-    <t>1,2</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Chưa có</t>
-  </si>
-  <si>
-    <t>999</t>
-  </si>
-  <si>
-    <t>2022-09-21</t>
-  </si>
-  <si>
-    <t>9999</t>
-  </si>
-  <si>
-    <t>45.png</t>
-  </si>
-  <si>
-    <t>2022-09-16</t>
-  </si>
-  <si>
-    <t>23456@gmail.com</t>
-  </si>
-  <si>
-    <t>Phúc Yên, Vĩnh Phúc</t>
-  </si>
-  <si>
-    <t>Khoa học máy tính</t>
-  </si>
-  <si>
-    <t>Ban Đào Tạo</t>
-  </si>
-  <si>
-    <t>Trưởng Ban</t>
-  </si>
-  <si>
-    <t>99999</t>
-  </si>
-  <si>
-    <t>2022-09-08</t>
   </si>
   <si>
     <t>999213</t>
@@ -559,7 +565,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -637,29 +643,29 @@
       <c r="F2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>16</v>
+      <c r="H2" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="O2" s="0" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2" s="0" t="b">
         <v>0</v>
@@ -672,6 +678,9 @@
       <c r="B3" s="0">
         <v>7</v>
       </c>
+      <c r="C3" s="0" t="s">
+        <v>27</v>
+      </c>
       <c r="D3" s="0" t="s">
         <v>18</v>
       </c>
@@ -682,25 +691,25 @@
         <v>20</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J3" s="0">
         <v>12</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O3" s="0" t="b">
         <v>0</v>
@@ -726,25 +735,25 @@
         <v>20</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J4" s="0">
         <v>12</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O4" s="0" t="b">
         <v>0</v>
@@ -770,25 +779,25 @@
         <v>20</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J5" s="0">
         <v>12</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O5" s="0" t="b">
         <v>0</v>
@@ -814,25 +823,25 @@
         <v>20</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="J6" s="0">
         <v>12</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O6" s="0" t="b">
         <v>0</v>
@@ -846,10 +855,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>18</v>
@@ -858,28 +867,28 @@
         <v>19</v>
       </c>
       <c r="F7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="J7" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O7" s="0" t="b">
         <v>0</v>
@@ -893,10 +902,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>18</v>
@@ -905,28 +914,28 @@
         <v>19</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="K8" s="0" t="s">
         <v>35</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O8" s="0" t="b">
         <v>0</v>
@@ -940,10 +949,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>18</v>
@@ -952,28 +961,28 @@
         <v>19</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N9" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O9" s="0" t="b">
         <v>0</v>
@@ -987,10 +996,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>18</v>
@@ -1002,25 +1011,25 @@
         <v>20</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="K10" s="0" t="s">
         <v>35</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O10" s="0" t="b">
         <v>0</v>
@@ -1034,10 +1043,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>18</v>
@@ -1046,28 +1055,28 @@
         <v>19</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="I11" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>34</v>
       </c>
       <c r="K11" s="0" t="s">
         <v>35</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O11" s="0" t="b">
         <v>0</v>
@@ -1081,10 +1090,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>18</v>
@@ -1093,31 +1102,31 @@
         <v>19</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>35</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N12" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O12" s="0" t="b">
         <v>0</v>
@@ -1131,43 +1140,43 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O13" s="0" t="b">
         <v>0</v>
@@ -1181,10 +1190,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>18</v>
@@ -1193,31 +1202,31 @@
         <v>19</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O14" s="0" t="b">
         <v>0</v>
@@ -1234,7 +1243,7 @@
         <v>5021</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>18</v>
@@ -1243,31 +1252,31 @@
         <v>19</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N15" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O15" s="0" t="b">
         <v>0</v>
@@ -1281,10 +1290,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>18</v>
@@ -1293,31 +1302,31 @@
         <v>19</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N16" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O16" s="0" t="b">
         <v>0</v>
@@ -1331,10 +1340,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>18</v>
@@ -1343,31 +1352,31 @@
         <v>19</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O17" s="0" t="b">
         <v>1</v>
@@ -1381,10 +1390,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>18</v>
@@ -1393,31 +1402,31 @@
         <v>19</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O18" s="0" t="b">
         <v>1</v>
@@ -1431,10 +1440,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>18</v>
@@ -1443,31 +1452,31 @@
         <v>19</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N19" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O19" s="0" t="b">
         <v>0</v>
@@ -1481,10 +1490,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>18</v>
@@ -1493,31 +1502,31 @@
         <v>19</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N20" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O20" s="0" t="b">
         <v>1</v>
@@ -1531,10 +1540,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>18</v>
@@ -1543,31 +1552,31 @@
         <v>19</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N21" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O21" s="0" t="b">
         <v>0</v>
@@ -1581,43 +1590,43 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N22" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O22" s="0" t="b">
         <v>1</v>
@@ -1631,10 +1640,10 @@
         <v>23</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>18</v>
@@ -1646,28 +1655,28 @@
         <v>20</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N23" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O23" s="0" t="b">
         <v>0</v>
@@ -1681,43 +1690,43 @@
         <v>24</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N24" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O24" s="0" t="b">
         <v>1</v>
@@ -1731,10 +1740,10 @@
         <v>25</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>18</v>
@@ -1746,28 +1755,28 @@
         <v>20</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N25" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O25" s="0" t="b">
         <v>1</v>
@@ -1781,43 +1790,43 @@
         <v>26</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="M26" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N26" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O26" s="0" t="b">
         <v>1</v>
@@ -1831,10 +1840,10 @@
         <v>27</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>18</v>
@@ -1843,31 +1852,31 @@
         <v>19</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O27" s="0" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Sửa lỗi Sửa thông tin
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/members.xlsx
+++ b/Hethongquanlylab/wwwroot/data/members.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\C#\Hethongquanlylab\Hethongquanlylab\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED408CA4-16B5-4CE5-BC0F-F072E51E659A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B00FE9-D720-494E-91D9-2AE2C0B0F34A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Key</t>
   </si>
@@ -75,10 +75,10 @@
     <t>Qua PTBT?</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Ngô Xuân Hinh.jpg</t>
+    <t>001100A2</t>
+  </si>
+  <si>
+    <t>Ngô Xuân Hinh.png</t>
   </si>
   <si>
     <t>Ngô Xuân Hinh</t>
@@ -90,10 +90,13 @@
     <t>2022-09-28</t>
   </si>
   <si>
-    <t>Khoa học máy tính 06</t>
-  </si>
-  <si>
-    <t>CNTT &amp; TT</t>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>Khoa học máy tính</t>
+  </si>
+  <si>
+    <t>Đại học Bách Khoa Hà Nội</t>
   </si>
   <si>
     <t>123456789</t>
@@ -102,40 +105,34 @@
     <t>23456@gmail.com</t>
   </si>
   <si>
+    <t>Phúc Thắng, Phúc Yên, Vĩnh Phúc</t>
+  </si>
+  <si>
+    <t>Chưa có</t>
+  </si>
+  <si>
+    <t>default.jpg</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>999</t>
+  </si>
+  <si>
+    <t>2022-09-21</t>
+  </si>
+  <si>
+    <t>9999</t>
+  </si>
+  <si>
+    <t>45.png</t>
+  </si>
+  <si>
+    <t>2022-09-16</t>
+  </si>
+  <si>
     <t>Phúc Yên, Vĩnh Phúc</t>
-  </si>
-  <si>
-    <t>Chưa có</t>
-  </si>
-  <si>
-    <t>default.jpg</t>
-  </si>
-  <si>
-    <t>1,2</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>999</t>
-  </si>
-  <si>
-    <t>2022-09-21</t>
-  </si>
-  <si>
-    <t>9999</t>
-  </si>
-  <si>
-    <t>45.png</t>
-  </si>
-  <si>
-    <t>2022-09-16</t>
-  </si>
-  <si>
-    <t>Khoa học máy tính</t>
-  </si>
-  <si>
-    <t>Đại học Bách Khoa Hà Nội</t>
   </si>
   <si>
     <t>Ban Đào Tạo</t>
@@ -565,7 +562,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -643,26 +640,29 @@
       <c r="F2" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="G2" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="H2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O2" s="0" t="b">
         <v>1</v>
@@ -679,7 +679,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>18</v>
@@ -691,7 +691,7 @@
         <v>20</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>29</v>
@@ -706,10 +706,10 @@
         <v>29</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O3" s="0" t="b">
         <v>0</v>
@@ -735,7 +735,7 @@
         <v>20</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>29</v>
@@ -750,10 +750,10 @@
         <v>29</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O4" s="0" t="b">
         <v>0</v>
@@ -779,7 +779,7 @@
         <v>20</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="I5" s="0" t="s">
         <v>29</v>
@@ -794,10 +794,10 @@
         <v>29</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O5" s="0" t="b">
         <v>0</v>
@@ -823,7 +823,7 @@
         <v>20</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>29</v>
@@ -838,10 +838,10 @@
         <v>29</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O6" s="0" t="b">
         <v>0</v>
@@ -858,7 +858,7 @@
         <v>30</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>18</v>
@@ -870,7 +870,7 @@
         <v>31</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>29</v>
@@ -885,10 +885,10 @@
         <v>29</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O7" s="0" t="b">
         <v>0</v>
@@ -917,25 +917,25 @@
         <v>34</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="L8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="M8" s="0" t="s">
+      <c r="N8" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="N8" s="0" t="s">
-        <v>38</v>
       </c>
       <c r="O8" s="0" t="b">
         <v>0</v>
@@ -949,40 +949,40 @@
         <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>40</v>
-      </c>
       <c r="G9" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N9" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O9" s="0" t="b">
         <v>0</v>
@@ -996,10 +996,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>18</v>
@@ -1011,25 +1011,25 @@
         <v>20</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O10" s="0" t="b">
         <v>0</v>
@@ -1043,10 +1043,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>18</v>
@@ -1058,25 +1058,25 @@
         <v>34</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="L11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="M11" s="0" t="s">
+      <c r="N11" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="N11" s="0" t="s">
-        <v>38</v>
       </c>
       <c r="O11" s="0" t="b">
         <v>0</v>
@@ -1090,43 +1090,43 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="0" t="s">
+      <c r="G12" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="0" t="s">
+      <c r="K12" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="M12" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="L12" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="M12" s="0" t="s">
+      <c r="N12" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="N12" s="0" t="s">
-        <v>38</v>
       </c>
       <c r="O12" s="0" t="b">
         <v>0</v>
@@ -1140,43 +1140,43 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="0" t="s">
+      <c r="E13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="G13" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O13" s="0" t="b">
         <v>0</v>
@@ -1190,43 +1190,43 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>51</v>
-      </c>
       <c r="G14" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O14" s="0" t="b">
         <v>0</v>
@@ -1243,7 +1243,7 @@
         <v>5021</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>18</v>
@@ -1252,31 +1252,31 @@
         <v>19</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N15" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O15" s="0" t="b">
         <v>0</v>
@@ -1290,10 +1290,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>18</v>
@@ -1305,28 +1305,28 @@
         <v>34</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N16" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O16" s="0" t="b">
         <v>0</v>
@@ -1340,43 +1340,43 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="D17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="0" t="s">
+      <c r="G17" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="L17" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="M17" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="G17" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="I17" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="J17" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="L17" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="M17" s="0" t="s">
-        <v>56</v>
-      </c>
       <c r="N17" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O17" s="0" t="b">
         <v>1</v>
@@ -1390,43 +1390,43 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="G18" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O18" s="0" t="b">
         <v>1</v>
@@ -1440,43 +1440,43 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>60</v>
-      </c>
       <c r="G19" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N19" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O19" s="0" t="b">
         <v>0</v>
@@ -1490,43 +1490,43 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="D20" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>63</v>
-      </c>
       <c r="G20" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N20" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O20" s="0" t="b">
         <v>1</v>
@@ -1540,10 +1540,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>18</v>
@@ -1552,31 +1552,31 @@
         <v>19</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N21" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O21" s="0" t="b">
         <v>0</v>
@@ -1590,43 +1590,43 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="E22" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N22" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O22" s="0" t="b">
         <v>1</v>
@@ -1640,10 +1640,10 @@
         <v>23</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>67</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>18</v>
@@ -1655,28 +1655,28 @@
         <v>20</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N23" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O23" s="0" t="b">
         <v>0</v>
@@ -1690,43 +1690,43 @@
         <v>24</v>
       </c>
       <c r="B24" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="E24" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N24" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O24" s="0" t="b">
         <v>1</v>
@@ -1740,10 +1740,10 @@
         <v>25</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>18</v>
@@ -1755,28 +1755,28 @@
         <v>20</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N25" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O25" s="0" t="b">
         <v>1</v>
@@ -1790,43 +1790,43 @@
         <v>26</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="E26" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M26" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N26" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O26" s="0" t="b">
         <v>1</v>
@@ -1843,7 +1843,7 @@
         <v>30</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>18</v>
@@ -1852,31 +1852,31 @@
         <v>19</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O27" s="0" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Sửa một số lỗi model
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/members.xlsx
+++ b/Hethongquanlylab/wwwroot/data/members.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Key</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>8.png</t>
+  </si>
+  <si>
+    <t>ds33</t>
   </si>
 </sst>
 </file>
@@ -559,7 +562,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
@@ -1885,6 +1888,56 @@
         <v>0</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" s="0">
+        <v>28</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="K28" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="L28" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="M28" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="N28" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="O28" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="P28" s="0" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>